<commit_message>
update paper to v4
</commit_message>
<xml_diff>
--- a/doc/实验数据.xlsx
+++ b/doc/实验数据.xlsx
@@ -31,10 +31,6 @@
   </si>
   <si>
     <t>mogb-dt-500-0.06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOGB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -79,6 +75,10 @@
   </si>
   <si>
     <t>sklearn-ada-dt-500-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOGB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12404,11 +12404,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="253161496"/>
-        <c:axId val="253544936"/>
+        <c:axId val="256932040"/>
+        <c:axId val="257821360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="253161496"/>
+        <c:axId val="256932040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12514,7 +12514,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253544936"/>
+        <c:crossAx val="257821360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -12524,7 +12524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253544936"/>
+        <c:axId val="257821360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.58000000000000007"/>
@@ -12640,7 +12640,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253161496"/>
+        <c:crossAx val="256932040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20379,11 +20379,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="417208936"/>
-        <c:axId val="253349320"/>
+        <c:axId val="256891744"/>
+        <c:axId val="256893152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="417208936"/>
+        <c:axId val="256891744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20489,7 +20489,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253349320"/>
+        <c:crossAx val="256893152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20499,7 +20499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253349320"/>
+        <c:axId val="256893152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.57000000000000006"/>
@@ -20615,7 +20615,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417208936"/>
+        <c:crossAx val="256891744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20935,11 +20935,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="253619216"/>
-        <c:axId val="253560928"/>
+        <c:axId val="257560840"/>
+        <c:axId val="257561864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253619216"/>
+        <c:axId val="257560840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20982,7 +20982,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253560928"/>
+        <c:crossAx val="257561864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20990,7 +20990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253560928"/>
+        <c:axId val="257561864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.47000000000000003"/>
@@ -21105,7 +21105,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253619216"/>
+        <c:crossAx val="257560840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21246,11 +21246,11 @@
         </c:dLbls>
         <c:gapWidth val="70"/>
         <c:overlap val="-4"/>
-        <c:axId val="252178080"/>
-        <c:axId val="252179256"/>
+        <c:axId val="257771896"/>
+        <c:axId val="255813296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252178080"/>
+        <c:axId val="257771896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21293,7 +21293,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252179256"/>
+        <c:crossAx val="255813296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21301,7 +21301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252179256"/>
+        <c:axId val="255813296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21411,7 +21411,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252178080"/>
+        <c:crossAx val="257771896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27597,11 +27597,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="252180040"/>
-        <c:axId val="252180432"/>
+        <c:axId val="257875888"/>
+        <c:axId val="257876280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="252180040"/>
+        <c:axId val="257875888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27703,7 +27703,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252180432"/>
+        <c:crossAx val="257876280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27712,7 +27712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252180432"/>
+        <c:axId val="257876280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.37000000000000005"/>
@@ -27827,7 +27827,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252180040"/>
+        <c:crossAx val="257875888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
@@ -28061,11 +28061,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254004784"/>
-        <c:axId val="254005176"/>
+        <c:axId val="257879024"/>
+        <c:axId val="257878240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254004784"/>
+        <c:axId val="257879024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28108,7 +28108,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254005176"/>
+        <c:crossAx val="257878240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28116,7 +28116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254005176"/>
+        <c:axId val="257878240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28167,7 +28167,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254004784"/>
+        <c:crossAx val="257879024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28372,11 +28372,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254005960"/>
-        <c:axId val="254006352"/>
+        <c:axId val="257879808"/>
+        <c:axId val="257880200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254005960"/>
+        <c:axId val="257879808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28473,7 +28473,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254006352"/>
+        <c:crossAx val="257880200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28481,7 +28481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254006352"/>
+        <c:axId val="257880200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28587,7 +28587,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254005960"/>
+        <c:crossAx val="257879808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28792,11 +28792,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="254007136"/>
-        <c:axId val="254007528"/>
+        <c:axId val="257880984"/>
+        <c:axId val="257881376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254007136"/>
+        <c:axId val="257880984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28894,7 +28894,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254007528"/>
+        <c:crossAx val="257881376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28902,7 +28902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254007528"/>
+        <c:axId val="257881376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29008,7 +29008,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254007136"/>
+        <c:crossAx val="257880984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -34016,7 +34016,7 @@
   <dimension ref="A1:W510"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B497" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="H510" sqref="H510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -34043,25 +34043,25 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
       <c r="V1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" t="s">
         <v>6</v>
-      </c>
-      <c r="W1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -69637,7 +69637,7 @@
     </row>
     <row r="506" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G506" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H506" s="1">
         <v>0.55901900000000004</v>
@@ -69645,7 +69645,7 @@
     </row>
     <row r="507" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G507" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H507" s="1">
         <v>0.52135632601199999</v>
@@ -69653,7 +69653,7 @@
     </row>
     <row r="508" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G508" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H508" s="1">
         <v>0.54835607830999999</v>
@@ -69661,7 +69661,7 @@
     </row>
     <row r="509" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G509" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H509" s="1">
         <v>0.54014799999999996</v>
@@ -69669,7 +69669,7 @@
     </row>
     <row r="510" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G510" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H510" s="1">
         <v>0.50672989044000005</v>
@@ -70424,7 +70424,7 @@
         <v>12750</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
@@ -70459,7 +70459,7 @@
         <v>16169</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>